<commit_message>
namespaces renamed for template/writers (code)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0c0cf5bc-9b4a-42a2-b709-c65ecfa4da8a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c222706e-4334-4488-8c96-f896f1afdde3}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2323b20-3bb2-4523-b846-c9781bfdc72d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{76db2eb3-ee99-4b28-8ecf-e151c9c4f326}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{71822a26-58c8-4cd8-8e05-75f761f8c03e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{98f69473-989a-4ab5-bac2-8af5664115de}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{adf51470-ba49-4344-8020-e715293b54a6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{95873722-9872-4fa2-810a-72d304fb9fbf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1a1671cf-dab8-4e9d-915b-17d1880f7aff}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c465f360-7abe-4e05-9196-4131d12ff823}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{db3b0b6c-bd68-4c95-8c2e-32c7a732c511}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1e7c2fb4-9478-451f-b700-d35618665370}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c5995afe-91d2-4320-81e8-9d5058630b81}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2ecd71a-26bf-4d3b-99c3-b0afa753dcae}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e40e4b74-63e6-4d12-aa82-756037c7749e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ef8791b7-5871-417b-8743-17e5b7f6d174}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cbdd3312-0b46-42b3-b9cf-505986579e5c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4e95fa93-0281-4d27-8a89-5fa3b9047254}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a98a2c4d-a9dc-4694-a949-e32bc9463da7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d4d8bcc5-8470-478c-b5d9-3891d66e7e96}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c65ef08b-5cb0-4a98-83e5-eecad1b4d4ca}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cae0178a-9791-4e02-ac62-1e74322476ea}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{46db098c-2ec6-40fa-adef-b503a2c29715}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2eb9d793-e209-421c-8c5c-efe1f4c363d7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{93006f23-06fb-44d0-827a-4f739c1d2f90}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1f46a624-696e-4d19-bed2-a0c285c5783d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6de550d0-1a21-4c96-887c-48730f325119}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cbd30935-b946-4543-966e-9f24013e4acd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5e2e8685-a19d-4cfb-8142-522eb42abad8}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8b9a19ec-a21b-485d-96e1-389fe76189a0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{217c4a20-e843-4c67-b344-c855991a0cad}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9eafa994-6592-4db7-909f-c5a810e2c9d7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{56cbcb7a-93d4-4e96-abeb-ff1033ddc8f0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{724eee2f-c546-4f5d-a237-a122258dc0fa}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d3ab7465-a29e-43b8-8553-80c021f78567}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{238cdc20-ca80-40b5-9cde-5ac6d17c17bf}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e9a86dd9-aba4-4fe8-a05d-1a4ab55423e8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bdbc8556-9147-4a01-9dfd-6c37cbd4e772}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{383640a8-41a2-400d-86e5-135326a016bd}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{152569d7-6026-4fc5-8b1d-96568c6c5d00}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1bf08574-f176-460f-a893-66ce5651e3b3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{84e965e9-5b76-4948-a94a-d39c57a6e32c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b5bf2b7f-d738-44f4-a29a-d2470102dbc2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d50f7f02-f9c0-403a-aea1-c13e3f8fae47}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{911ace12-6dc1-479b-a14e-02161e80181e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{660d9ed7-804e-495b-b3c7-bc2f49809757}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8e0f8093-135d-454d-9211-b71c455a9ded}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{421158e8-2939-435f-98d6-0716117ca032}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e7f75b69-0568-4992-a1d4-393e19872381}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f13cab3e-e564-411d-8f0a-86b5980bab22}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7c7c1cea-99ac-4417-b2cc-eba7832e2914}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0e5cec8a-9269-41ee-86b0-4d5b522c1c2a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c3516647-5e55-4436-a801-94c64dc221b1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{722f2a72-dee8-4d27-81a9-806f4e78c2cd}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0785dfea-70f0-4daf-b416-916f54adf428}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ff77b6ca-b43b-48ac-8baa-db4bf9137911}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d3d235fc-2e78-4ae5-8555-1a741acb7e9b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c449f271-c8eb-4f5f-afe2-26d88eeda058}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b93c73de-2f1e-49bf-a426-c3d9f71b3f4a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7188efcf-2ed4-42c5-b107-3f38b4e15fed}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fc04164a-7e7a-4253-8e87-f0de9ca50a82}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{818eb68a-f60e-43b2-8f52-b3fce9840f41}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ade3169b-aab0-44f7-b5a2-b6dc61558129}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3be21839-01d8-4c4e-a7e9-2c727320bce4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Add Word Template Writer Sample (In progress..)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c222706e-4334-4488-8c96-f896f1afdde3}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d297c814-a3fe-44cc-8b5b-c0ccf9e0bc07}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{76db2eb3-ee99-4b28-8ecf-e151c9c4f326}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5cf258fc-7ef6-4522-b19e-0baa8653973a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{98f69473-989a-4ab5-bac2-8af5664115de}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1aaac6de-c65e-4562-9e28-05fe3acba378}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{95873722-9872-4fa2-810a-72d304fb9fbf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a75a19d0-bda8-4ef2-af52-5d396900df70}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c465f360-7abe-4e05-9196-4131d12ff823}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c7b0d3d6-95ed-46bd-beb7-55aa6d54b53c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1e7c2fb4-9478-451f-b700-d35618665370}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{646f678d-356b-4c0a-92a7-f0e31ff1d6a6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2ecd71a-26bf-4d3b-99c3-b0afa753dcae}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a14fc6a0-3656-4113-8aa9-0b27c500c68d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ef8791b7-5871-417b-8743-17e5b7f6d174}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{740a50b9-86c4-4081-a6c7-743724d9717c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4e95fa93-0281-4d27-8a89-5fa3b9047254}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4d2cec6e-0051-41e1-8ade-2cfb53b90e83}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d4d8bcc5-8470-478c-b5d9-3891d66e7e96}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5f54c610-a77b-41c7-9584-6cb912661108}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cae0178a-9791-4e02-ac62-1e74322476ea}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2a65b8ca-aa57-41e0-b9bd-8fdd9c61ab5c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2eb9d793-e209-421c-8c5c-efe1f4c363d7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2f1dc59f-9235-4ad9-a452-0c69faad2fc4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1f46a624-696e-4d19-bed2-a0c285c5783d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{47912852-66c2-417f-aba4-5415c578df61}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cbd30935-b946-4543-966e-9f24013e4acd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9f4d58d0-5dcf-4c15-a3f6-33dfbb0447f0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8b9a19ec-a21b-485d-96e1-389fe76189a0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{764199eb-b3b7-405b-96e6-e10b7d619da2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9eafa994-6592-4db7-909f-c5a810e2c9d7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cff7f967-2aee-41af-aa9b-ebb6b6b4059c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{724eee2f-c546-4f5d-a237-a122258dc0fa}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d352ccbd-267b-429c-8272-93761db58ecf}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{238cdc20-ca80-40b5-9cde-5ac6d17c17bf}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8ecd502e-5ca0-4f3f-a9ec-e88ae261e51e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bdbc8556-9147-4a01-9dfd-6c37cbd4e772}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{822531bb-c6b9-4dcd-92e8-371dad483d2b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{152569d7-6026-4fc5-8b1d-96568c6c5d00}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{74bd5e96-fecd-48a5-b432-91848528dc2c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{84e965e9-5b76-4948-a94a-d39c57a6e32c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9b7c9abe-9092-4aaf-8901-d59e8f3b274f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d50f7f02-f9c0-403a-aea1-c13e3f8fae47}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1b39164e-74f6-4fcc-9811-7cfd5256b0cc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{660d9ed7-804e-495b-b3c7-bc2f49809757}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{88909f82-f6c1-4a28-a215-f133b6f1f859}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{421158e8-2939-435f-98d6-0716117ca032}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ff4a95a2-c5dd-4372-8c29-d821b3bec305}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f13cab3e-e564-411d-8f0a-86b5980bab22}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{58d5d96c-3dd6-4871-92af-1ab8f5397431}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0e5cec8a-9269-41ee-86b0-4d5b522c1c2a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7562f4c8-aecb-44be-896d-9859ee591972}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{722f2a72-dee8-4d27-81a9-806f4e78c2cd}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9ca9d337-42dd-4426-b6de-b82afef79375}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ff77b6ca-b43b-48ac-8baa-db4bf9137911}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{31b55f9f-4a1a-4430-852c-4db804a2e461}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c449f271-c8eb-4f5f-afe2-26d88eeda058}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{57b5b601-6089-4104-badd-7eb3a7f6d016}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7188efcf-2ed4-42c5-b107-3f38b4e15fed}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{97971e8a-2ab4-4f4d-96e2-56389aa67cb3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{818eb68a-f60e-43b2-8f52-b3fce9840f41}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ef0eb6ea-4924-4a02-8797-0cbfba2faccf}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3be21839-01d8-4c4e-a7e9-2c727320bce4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f04a2783-cc4e-4874-a8b7-c7219eedb033}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Finished Integration Mailing Functionality (Word), see template sample in iTinExportEngineSamples
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{96f5e0b3-8491-4140-9abc-02f928d21993}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2cf4f41c-4f07-41a0-a23d-273a94a39134}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6c49d0f2-841d-4705-8d1a-cdc86ade6535}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9b23f9fd-bbde-41d7-bb51-9bc0dbd2e487}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4369b989-8cd5-437f-834a-5374890073ee}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2e62dfe9-2559-4211-bf6a-458348339e3f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8128b69b-bcc3-401c-8b98-8e666b75ee07}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{87189e3d-1e5a-4d4f-97f9-d9465884bb55}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5b99883f-621f-4179-904d-42e5122dc559}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9e750e6f-a65c-40b1-8989-4a51baee24e0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f200fd02-016d-426a-97da-183d95a879be}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c3869f08-e744-4bf0-92cc-f81e55e6151c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d66cb106-ab4f-4c39-aa8e-8f10387e76d6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4583309b-a233-4eef-b979-dec5c5faf7c3}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ef2119a-a954-444b-aae4-ef0774476d77}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{29361e75-b189-4444-8fd5-e9460dacf5a2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{19c6867c-ee52-4aa4-9d66-58ed10ca1fc3}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5e5b15a0-73f1-49dc-a15c-9faf239fb2af}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{39a36efb-f325-4f14-88e0-4473e1d170ff}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d9cc90d0-79a5-4e49-9ba9-bd93124248a5}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{92821a57-d91a-4b73-af47-3cd3c68b32e1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{765d6b0b-7c4c-4715-a0ac-ce0593122c59}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{684a213e-1a5a-4feb-954e-c3a4d2794169}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{37bf21c3-4676-43b7-b250-0ba9635fc32a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{051f17a6-2e76-44e5-a437-a400f10d3229}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{49116c4e-0912-4303-97d9-c6c46cced832}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d9f9c4fe-67a6-4cca-8636-cae40640d891}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{405ad76f-d294-4050-b123-3d31ae672a4e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{71234051-2d8d-4500-b4b6-7b75b52a253b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d225585b-ea2d-4233-a2c2-2763e09b52f3}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aae51ceb-3a25-4beb-8931-3a4dedc4244c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d8ea1e1e-72e8-49a4-9339-a8250fd00d4d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d6be6313-de7f-4428-b1c0-10668b29e283}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9aadf89b-9d67-42a0-b50d-47d166bd6344}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{564073ca-acdc-472e-af81-95fc93f88ff7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{210a1ba7-cb6b-4d5e-a7f6-46cda8502857}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{72aba9df-3cf9-42b6-a17a-b8ec2587a4c1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fc40d9b4-56d4-4768-8f0e-79cb6cde98d7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9ac24293-527c-4ada-ae14-29c60282f595}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4b25ab6a-a6c4-4099-84f8-447e1dc33cb4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0e4036dd-e22c-4b5f-91d4-746d7e617e4e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ed02a8af-a195-47e5-94e3-6b8935894cdc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a14a59cf-7603-4521-9fd7-ac9b723f8b34}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e7906c55-8fc8-4256-aa44-fc49b43d701e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bb68a008-a4ae-4aad-8d3e-c300fbba8c84}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{56018cc9-2655-47e5-a4a5-d931b128b726}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b099de74-7bcf-41ce-9739-2b28ae56e762}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{675e4bf0-a921-44af-a1c0-12cce42518a5}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e453dd76-0aec-49f4-9385-5716c54241ea}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a8c03d81-b716-4e4a-91a1-914d947554f8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e1543a21-edfc-40be-af8b-c9e17fe18cc9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0b2cf644-b779-4760-b2f3-b148b8ee03d1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e37b59b2-e915-4a5b-9ccc-d3b769b59f11}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8216427d-a977-45c8-b2af-165b862114a3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8becfe01-f192-429a-ad67-e7f1ea0799d2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{25868996-d0a7-4b1b-bdd1-8803633741ee}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b1ce1415-883b-46f5-9d5c-67e8a756046b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{303d6713-1233-4bc8-b7c6-925bd754b018}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9fda15bf-2643-402c-97a4-9aafb22f9afb}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{97cdfb34-caaf-498b-8dbc-7f126ffd522a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a092e2c4-0479-47d2-96fb-6c2849f14519}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{80d93038-7ede-425a-875d-aa7521b2ad29}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e7763633-5d7b-41f1-8832-23aa26536211}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e3f07b47-acc9-4b2a-b186-f2d21445e7fc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Minor changes in CsvWriter
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{60d70a2c-6cd4-4373-bc9a-587a80ab193a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{69306ba9-4cd8-4f96-8e3f-27a379a433cf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a49eebcb-0882-4083-9ce1-f061f820a9aa}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8af8573b-2db1-4fdd-8100-bc7defd5ac4f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3bbcfa19-1b08-4da4-9672-856b87c90ac7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4e4266f5-5817-4981-950a-f0139fd18e81}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7a99fef2-662a-4203-9fec-503574edabe1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{de220f33-2bf7-4109-b92b-11e164079fb4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{15838dc8-ccee-452d-8366-3166e83d749a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0647ad79-75ed-43cd-ad2a-0d211afb6f7c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e9a24965-ae56-49e5-995e-7d4d808aa121}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{52875759-4375-4728-aea6-28005b909625}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4fc5132e-6f77-474c-a2ee-7d97b7c02212}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b04d90c2-964e-4b79-ae57-bc48a36289cf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d875b32a-3f2c-497e-937e-76f02eb4fc99}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9b7b68bd-b567-4502-8c7b-7d769db2a82c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f8d25531-91b4-49a2-85db-eb07d4f048c3}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{942dce55-4669-4442-ae2b-06df9fdb1ea2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{795ade6d-d521-4cf0-a8b3-ab1dc21a5014}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{14b3cc43-59c9-44bb-b099-9efdb3ef788c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ece708b4-574b-4f2e-acd9-49f624ce9384}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6273fe66-f3d0-4800-b12d-7a88866d009c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d4e885be-41d0-4ae9-ba03-b5679685ce3d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{45e7de05-1f5a-418b-ac22-1e16e604009f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6007ce20-c116-40b8-a5c8-d3e635c31511}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0d50324d-ade9-4815-a089-2e446b1cec72}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e5535764-b114-4b6b-afbe-cf100f4ea8ec}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2ce44731-9dba-4f6d-b5b6-f39fb903d076}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{52fa0a6c-47a0-4bfe-b16b-3f654f3de112}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7e4e0b60-7e68-4d00-8765-a2168a034214}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e93384ea-8abf-408b-84fa-c860803b3a40}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e5bc9c2c-1d9d-4d4e-a39e-07662dd875e1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{75a6335a-b43e-47d0-bb73-156545744a5e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d99e22b1-cdaa-4b57-8343-2716e82bed6a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fa0006b0-daca-4a5e-a562-19e779f47fc8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d4ebb96c-8fb6-41e9-993d-464b27ce1744}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e7950d23-75eb-47b4-bfdd-ef744768da42}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{abe010e4-bdb3-4f98-b0ab-e74cace236ec}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{784a5a6e-d814-4e53-9553-7294e71c2764}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fd16e555-7edb-4141-869b-137f05c541bc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{474c2743-5271-4adb-a65b-8696d008bdd1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ba2e3a25-123c-4537-a095-d4949fea12f0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fb1ead01-0129-448b-866e-28ccef5972d1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e821a3d0-c496-440c-82bc-692cc2b7fe5a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{11ffdb33-a0f7-4def-9a56-24fa6949bbda}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a9aeaa9d-5597-489a-9095-c23f14528bef}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{015d41bc-bf21-41c1-9d92-502f30560e9a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{33e0ee7b-9472-4739-b105-59da0d15d5ce}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{64a9e1c3-bc2d-4a72-91ac-ab08a775d72b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4bc62593-6e08-4f7a-bec4-072cde8a6696}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9be49ade-2b35-4716-aa36-e6feaaa8d426}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ccaa632c-f8d7-4138-a4d0-b433da40f1ae}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{65e3758a-93ee-4293-a539-770251ebf85c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2245c7d8-3c2b-4430-957d-264172842fde}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{dcd0c224-0499-4c82-bb06-5b9bf293bea3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{094239e1-3f72-426a-96c3-a25946fe1f46}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6a792eba-5a38-47b8-99d4-f212bcfe555a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{04b0108e-bc64-4145-816e-7235f3c8ced4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{26372cf6-b00b-4443-b6a8-e1a7c11bce73}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{98034f7a-ccd4-4f0a-b765-2cc65415f88b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a5b40df7-19e5-46b1-88d7-7702ad86f07e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f2749016-6a07-456d-9746-7e673a0a7b31}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f8fbd004-8067-465d-a683-e49086086704}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{59f99e3a-2728-4b5b-844b-7dc2958a61b3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Update native SqlWriter, add " ' " delimiter for text fields, numeric decimal/float values format correctly, datetime in progress...
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{69306ba9-4cd8-4f96-8e3f-27a379a433cf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1c780267-307e-497c-b903-b9aae7ccb49d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8af8573b-2db1-4fdd-8100-bc7defd5ac4f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fe9b5bae-a060-4590-9458-d8af63e6741d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4e4266f5-5817-4981-950a-f0139fd18e81}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7e705b68-b850-41b6-9590-72f293f035c9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{de220f33-2bf7-4109-b92b-11e164079fb4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aa611393-1a99-4021-91f5-c878453b0248}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0647ad79-75ed-43cd-ad2a-0d211afb6f7c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1d187438-7032-432c-9c19-cbfd8728cff4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{52875759-4375-4728-aea6-28005b909625}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{dcc5fb53-6a68-4967-85fc-b0ba9cecb0a9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b04d90c2-964e-4b79-ae57-bc48a36289cf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{28858f90-83a0-4682-81b8-e4e30564cedf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9b7b68bd-b567-4502-8c7b-7d769db2a82c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2fe551f2-456a-4071-95af-e7b6f198c4bd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{942dce55-4669-4442-ae2b-06df9fdb1ea2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{222cb4b4-fae0-4f8f-8b74-8d6f29a4cb1c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{14b3cc43-59c9-44bb-b099-9efdb3ef788c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d928f499-5c0f-411b-9c15-90b7e46e8452}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6273fe66-f3d0-4800-b12d-7a88866d009c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f06ac5ee-8c87-4bd5-a89d-9334154ce497}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{45e7de05-1f5a-418b-ac22-1e16e604009f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b4c7e370-d991-4275-82e5-9c01f0840023}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0d50324d-ade9-4815-a089-2e446b1cec72}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b996762b-4757-4472-a0e8-ff10f5dd34ae}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2ce44731-9dba-4f6d-b5b6-f39fb903d076}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{98bf4cae-b054-413a-bc9a-3f2929f5f360}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7e4e0b60-7e68-4d00-8765-a2168a034214}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a6a7ab03-d6f2-4c33-ac51-1cc504d7c9eb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e5bc9c2c-1d9d-4d4e-a39e-07662dd875e1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{479c7e9d-bf0b-4c26-889a-24c94f6b38a9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d99e22b1-cdaa-4b57-8343-2716e82bed6a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{43f78cc6-b9fb-4064-b088-a363d74f4dc1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d4ebb96c-8fb6-41e9-993d-464b27ce1744}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7698044b-94b3-4355-a362-8eab4e9fc44c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{abe010e4-bdb3-4f98-b0ab-e74cace236ec}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{21cdbb16-0ece-4ae9-a3dc-56b127190353}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fd16e555-7edb-4141-869b-137f05c541bc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e6f74c6e-f507-4ba6-9950-a3d2db994581}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ba2e3a25-123c-4537-a095-d4949fea12f0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9fdaff7d-e27a-45ad-b46b-e2d763ce48b2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e821a3d0-c496-440c-82bc-692cc2b7fe5a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{afbfa7ce-9f9e-4dc2-a410-9cb8845e80d0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a9aeaa9d-5597-489a-9095-c23f14528bef}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{46810464-9a68-49c5-9c6e-a01462528af5}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{33e0ee7b-9472-4739-b105-59da0d15d5ce}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ca5d835-18ce-4b38-8af3-4c063403fb29}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4bc62593-6e08-4f7a-bec4-072cde8a6696}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{83d6d4b7-69ba-4c2b-8960-a6d6474ec4b4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ccaa632c-f8d7-4138-a4d0-b433da40f1ae}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5f8b2757-aecb-47b3-a9b9-d39f90a25690}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2245c7d8-3c2b-4430-957d-264172842fde}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e89ad885-1c04-4c0c-bd78-7f72d0ff034e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{094239e1-3f72-426a-96c3-a25946fe1f46}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2e344410-b3fd-48b3-afc9-f15af73ddba5}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{04b0108e-bc64-4145-816e-7235f3c8ced4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8dafca29-4652-4eab-9b73-a0977d9a79af}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{98034f7a-ccd4-4f0a-b765-2cc65415f88b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b87457d7-d657-4023-bb7a-0447e4dd61be}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f2749016-6a07-456d-9746-7e673a0a7b31}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8d7a513a-ec0c-49fe-9810-c699ad4e8694}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{59f99e3a-2728-4b5b-844b-7dc2958a61b3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9051f754-6b83-40f0-9a8d-c02ffb6742ca}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Partial support of blocklines for Markdown writer
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1c780267-307e-497c-b903-b9aae7ccb49d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{74527846-acdf-4ad9-ad2d-8090c01b73cb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fe9b5bae-a060-4590-9458-d8af63e6741d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d5f008e8-e2c5-41fa-90f7-0184a4deb632}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7e705b68-b850-41b6-9590-72f293f035c9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c5b944bb-5a01-4fe6-82ff-501af027c3d8}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aa611393-1a99-4021-91f5-c878453b0248}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4704e447-f0de-4f06-96f2-df3675764f3e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1d187438-7032-432c-9c19-cbfd8728cff4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a66ffd57-3e8f-41a2-b946-a69365326c69}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{dcc5fb53-6a68-4967-85fc-b0ba9cecb0a9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2ca82542-eb97-4026-8eeb-d5bc9dee04da}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{28858f90-83a0-4682-81b8-e4e30564cedf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e25dc8c0-c71c-4a54-bc1c-4029006f4308}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2fe551f2-456a-4071-95af-e7b6f198c4bd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c0cad9f9-1a38-4c96-bd0e-9f874cdedbcb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{222cb4b4-fae0-4f8f-8b74-8d6f29a4cb1c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d8e08bfb-5589-410a-84f3-1cc8f3b29f9d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d928f499-5c0f-411b-9c15-90b7e46e8452}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{74c17e8c-81b3-4f5b-a4f0-4c26543ba0ad}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f06ac5ee-8c87-4bd5-a89d-9334154ce497}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{20fd8f0c-f9bb-4376-a19e-2ee66772b039}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b4c7e370-d991-4275-82e5-9c01f0840023}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c37455c4-a10d-4a17-93ea-0fb23d7f566d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b996762b-4757-4472-a0e8-ff10f5dd34ae}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d28aa2f4-934d-4161-bd38-8d7dca7757dd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{98bf4cae-b054-413a-bc9a-3f2929f5f360}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2cdb15ef-0c09-406d-8edd-98a861797226}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a6a7ab03-d6f2-4c33-ac51-1cc504d7c9eb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{de6c80f8-58ef-41ed-9ea1-eede92d62b61}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{479c7e9d-bf0b-4c26-889a-24c94f6b38a9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f58d0958-2f8b-454e-80a5-37b267cd424c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{43f78cc6-b9fb-4064-b088-a363d74f4dc1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{14deb8d1-0afd-4619-a35a-ac625e45e6a8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7698044b-94b3-4355-a362-8eab4e9fc44c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c9b04c95-ee5a-4835-aafa-9462313f9d31}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{21cdbb16-0ece-4ae9-a3dc-56b127190353}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{991a3d04-351a-412d-ab82-01b43d3c65b3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e6f74c6e-f507-4ba6-9950-a3d2db994581}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ed527897-dbf3-4db5-a2ec-91ce4db2c4cd}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9fdaff7d-e27a-45ad-b46b-e2d763ce48b2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c22330bb-e588-4f03-857b-27c70f69d799}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{afbfa7ce-9f9e-4dc2-a410-9cb8845e80d0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e48a29bd-0f8b-4245-ae8e-642bebf99f20}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{46810464-9a68-49c5-9c6e-a01462528af5}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{131e0b26-e110-44ff-b80c-caff6481b3d7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ca5d835-18ce-4b38-8af3-4c063403fb29}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c4ab533b-17e1-44b2-9237-ba98e7f6addc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{83d6d4b7-69ba-4c2b-8960-a6d6474ec4b4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6fd51e81-055c-449e-bf3b-b7917834ae5f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5f8b2757-aecb-47b3-a9b9-d39f90a25690}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{78d5099a-3945-4740-ba15-6df104b0b673}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e89ad885-1c04-4c0c-bd78-7f72d0ff034e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1e468dc5-fc84-4510-992f-f1e48ba16b2d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2e344410-b3fd-48b3-afc9-f15af73ddba5}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1a8b0b2d-65d7-46e8-8cf3-1961d8c699ac}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8dafca29-4652-4eab-9b73-a0977d9a79af}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9e38a182-1aa2-47e4-8578-540e2e2efc7b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b87457d7-d657-4023-bb7a-0447e4dd61be}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{436891e7-15f6-492d-b54d-2acd058d35eb}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8d7a513a-ec0c-49fe-9810-c699ad4e8694}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{44634c37-b6fe-475e-944c-336aead5f870}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9051f754-6b83-40f0-9a8d-c02ffb6742ca}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d56eb7c4-8e1f-4f74-a275-bb6c80a0a401}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Add markdown help (help folder) in sample project, prepare many changes and bug fixes in v2.0.1
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/writer/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{74527846-acdf-4ad9-ad2d-8090c01b73cb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d8d19288-73e0-447e-b585-b4646f99ebd1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d5f008e8-e2c5-41fa-90f7-0184a4deb632}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6d122d81-aa97-4573-b290-2e7c7864dec4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c5b944bb-5a01-4fe6-82ff-501af027c3d8}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e5d30d2e-5ee9-4975-83db-ee804ca29700}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4704e447-f0de-4f06-96f2-df3675764f3e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{79e302a7-6765-4ede-9f9a-f4ce6ba7bca2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a66ffd57-3e8f-41a2-b946-a69365326c69}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b067b308-fd94-4d90-82bb-aaa0d4f17fdc}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2ca82542-eb97-4026-8eeb-d5bc9dee04da}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{45865447-6a1f-4039-8d4f-eafa9d1f03d7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e25dc8c0-c71c-4a54-bc1c-4029006f4308}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6b66616b-be89-4654-afd5-be03680ad650}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c0cad9f9-1a38-4c96-bd0e-9f874cdedbcb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cc3e057b-8168-40cd-a6a3-4f0c94c21ddf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d8e08bfb-5589-410a-84f3-1cc8f3b29f9d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7032c0d3-bf7c-49a2-bfb2-408d0673f452}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{74c17e8c-81b3-4f5b-a4f0-4c26543ba0ad}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a1bc71b3-d005-4b22-b79a-ddb8bbde0604}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{20fd8f0c-f9bb-4376-a19e-2ee66772b039}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5d186d4a-e337-436d-ae12-951ea55aa1ef}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c37455c4-a10d-4a17-93ea-0fb23d7f566d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{566b7586-d12d-4972-ae63-05f0c0c497da}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d28aa2f4-934d-4161-bd38-8d7dca7757dd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c25450dd-1779-442c-875e-bac734eaf84e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2cdb15ef-0c09-406d-8edd-98a861797226}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b26cc427-50ce-4fad-a98a-f8e6561065b2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{de6c80f8-58ef-41ed-9ea1-eede92d62b61}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1cc49286-26c8-4c16-8ec5-0be8beb9ed67}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f58d0958-2f8b-454e-80a5-37b267cd424c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{923b86f6-0736-4979-a5f7-79c9a441f59d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{14deb8d1-0afd-4619-a35a-ac625e45e6a8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bf4816bb-054e-437b-bd65-bf380ecf7b8f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c9b04c95-ee5a-4835-aafa-9462313f9d31}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{31b1fbf2-8eae-4985-9430-da65fc4ec82b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{991a3d04-351a-412d-ab82-01b43d3c65b3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{59213f3e-8f85-4261-9179-9e41efba4841}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ed527897-dbf3-4db5-a2ec-91ce4db2c4cd}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5542fb39-a6f0-4d88-8df6-d09932156344}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c22330bb-e588-4f03-857b-27c70f69d799}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4eb9e1e6-01dd-4f0c-9409-a0e6b78606d4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e48a29bd-0f8b-4245-ae8e-642bebf99f20}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{848a6cb1-def4-4a75-829d-93bbb37acd1a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{131e0b26-e110-44ff-b80c-caff6481b3d7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2b6ecb9f-8582-483d-a021-98a27ab127f5}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c4ab533b-17e1-44b2-9237-ba98e7f6addc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f95da6c6-5a36-41ff-9e10-d26d384c7b14}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6fd51e81-055c-449e-bf3b-b7917834ae5f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9e3451ea-5c15-47b6-96f9-646998b5a9f8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{78d5099a-3945-4740-ba15-6df104b0b673}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cdf460db-15c7-4b09-95e5-10d90d991280}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1e468dc5-fc84-4510-992f-f1e48ba16b2d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0c19170d-6ee9-42d1-b5a0-f9e6cbb71f2b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1a8b0b2d-65d7-46e8-8cf3-1961d8c699ac}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cd6901d4-8cdb-4e6c-8d58-d817197fce54}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9e38a182-1aa2-47e4-8578-540e2e2efc7b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0035bbfb-a0b4-470f-915c-2522570640c2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{436891e7-15f6-492d-b54d-2acd058d35eb}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{db06459f-b207-4974-ac94-d75725a29c64}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{44634c37-b6fe-475e-944c-336aead5f870}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cd164c74-ad52-4a2c-bbfc-8c21e0710eee}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d56eb7c4-8e1f-4f74-a275-bb6c80a0a401}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e7ac0770-1fff-4481-845b-d3e35920d984}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>